<commit_message>
fix: member permissions; add: report formats fixed and implemented in sheet json
</commit_message>
<xml_diff>
--- a/resources/excel/PromoterWorkbook.xlsx
+++ b/resources/excel/PromoterWorkbook.xlsx
@@ -9,6 +9,7 @@
     <sheet state="visible" name="commissions_sheet" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="link_stats_sheet" sheetId="5" r:id="rId8"/>
     <sheet state="visible" name="referral_aggregate_sheet" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="member_sheet" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="71">
   <si>
     <t>purchase_table</t>
   </si>
@@ -147,6 +148,9 @@
     <t>total_commission</t>
   </si>
   <si>
+    <t>updated_at</t>
+  </si>
+  <si>
     <t>commission_table</t>
   </si>
   <si>
@@ -171,6 +175,12 @@
     <t>link_stats_table</t>
   </si>
   <si>
+    <t>link_name</t>
+  </si>
+  <si>
+    <t>Aditya's link</t>
+  </si>
+  <si>
     <t>ref_val</t>
   </si>
   <si>
@@ -193,6 +203,33 @@
   </si>
   <si>
     <t>total_purchases</t>
+  </si>
+  <si>
+    <t>member_table</t>
+  </si>
+  <si>
+    <t>member_id</t>
+  </si>
+  <si>
+    <t>Joan</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>joan@mail.com</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>admin, editor, viewer</t>
+  </si>
+  <si>
+    <t>editor</t>
+  </si>
+  <si>
+    <t>added_on</t>
   </si>
 </sst>
 </file>
@@ -346,6 +383,10 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1233,7 +1274,7 @@
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>13</v>
@@ -1277,7 +1318,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1327,7 +1368,7 @@
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>13</v>
@@ -1350,7 +1391,7 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>13</v>
@@ -1373,7 +1414,7 @@
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>13</v>
@@ -1387,16 +1428,16 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>13</v>
@@ -1463,7 +1504,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1536,7 +1577,7 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>13</v>
@@ -1544,20 +1585,20 @@
       <c r="C4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="7">
-        <v>80.4</v>
+      <c r="I4" s="8"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>13</v>
@@ -1565,45 +1606,43 @@
       <c r="C5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="8"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>52</v>
+      <c r="J5" s="8"/>
+      <c r="K5" s="7">
+        <v>80.4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0.0</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="7">
-        <v>9180.4</v>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>13</v>
@@ -1620,11 +1659,13 @@
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="K7" s="7">
+        <v>9180.4</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>13</v>
@@ -1645,22 +1686,43 @@
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="8"/>
+        <v>26</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.0</v>
+      </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="7" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1689,7 +1751,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1739,7 +1801,7 @@
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>13</v>
@@ -1780,12 +1842,12 @@
         <v>15</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>13</v>
@@ -1808,7 +1870,7 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>13</v>
@@ -1881,4 +1943,207 @@
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="17.63"/>
+    <col customWidth="1" min="9" max="9" width="16.25"/>
+    <col customWidth="1" min="11" max="11" width="45.63"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="8"/>
+      <c r="K7" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>